<commit_message>
Small datatier layer changes
</commit_message>
<xml_diff>
--- a/project/SystemDev/MoSCoW.xlsx
+++ b/project/SystemDev/MoSCoW.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Music player</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Public chat</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>Follow/subscribe</t>
@@ -523,7 +520,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F27"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,24 +553,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -581,10 +576,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -596,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -605,10 +600,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -618,7 +613,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3"/>
     </row>

</xml_diff>